<commit_message>
Changed excel for data analysis
</commit_message>
<xml_diff>
--- a/reports/Excels/1_Raw_Experiment.xlsx
+++ b/reports/Excels/1_Raw_Experiment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orelt\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orelt\projects\Sleep-Stage-Prediction-Classification-Using-Neural-ODE\reports\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9DD5666-A5F2-4802-8E6C-F56E721697E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51ADD097-59BC-4835-8BC4-2DE050E49B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30588" yWindow="-132" windowWidth="30984" windowHeight="16824" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -101,6 +101,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -253,7 +256,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
@@ -266,7 +269,10 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -554,7 +560,7 @@
   <dimension ref="B1:D18"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -717,10 +723,10 @@
       <c r="B15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="6">
         <v>0.6119</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="6">
         <v>0.62</v>
       </c>
     </row>
@@ -728,11 +734,11 @@
       <c r="B16" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="7">
         <f>AVERAGE(C2:C15)</f>
         <v>0.60086428571428574</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="7">
         <f>AVERAGE(D2:D15)</f>
         <v>0.55417142857142865</v>
       </c>
@@ -741,11 +747,11 @@
       <c r="B17" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="7">
         <f>MEDIAN(C2:C15)</f>
         <v>0.61775000000000002</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="7">
         <f>MEDIAN(D2:D15)</f>
         <v>0.57824999999999993</v>
       </c>
@@ -754,11 +760,11 @@
       <c r="B18" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="7">
         <f>_xlfn.STDEV.S(C2:C15)</f>
         <v>0.10256980817692148</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="7">
         <f>_xlfn.STDEV.S(D2:D15)</f>
         <v>8.4545358136432103E-2</v>
       </c>

</xml_diff>